<commit_message>
Support for 8D surface and least squares using correlation
</commit_message>
<xml_diff>
--- a/stockData.xlsx
+++ b/stockData.xlsx
@@ -4,12 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="daily" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="60min" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5min" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -464,11 +465,11 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="3" width="11.52"/>
   </cols>
@@ -600,557 +601,557 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="2" s="4">
+    <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0.1353339795254263</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0.02311614774525422</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0.002416155435321068</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.008756418689102752</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>-0.002386713597914154</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>0.003248142567883146</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>1.683741890070394e-11</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>1.365890513733459e-10</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>7.987578806672784e-06</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>-1.178914113291122</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>-0.008682686874265128</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>-0.4459318965908032</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>0.06639658324626443</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>-0.01219697570948368</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>0.008753731320656585</v>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>-0.006256505902792851</v>
+      </c>
+      <c r="R2" s="3" t="n">
+        <v>0.1817201811518735</v>
+      </c>
+      <c r="S2" s="3" t="n">
+        <v>0.2311367116934373</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>0.228938436374275</v>
+      </c>
+      <c r="U2" s="3" t="n">
+        <v>0.1764903635473043</v>
+      </c>
+      <c r="V2" s="3" t="n">
+        <v>-0.01775379962266861</v>
+      </c>
+      <c r="W2" s="3" t="n">
+        <v>0.179125441950419</v>
+      </c>
+      <c r="X2" s="3" t="n">
+        <v>0.00402048532970439</v>
+      </c>
+      <c r="Y2" s="3" t="n">
+        <v>0.01632217957565525</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
           <t>NIO</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>0.1409390629431482</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>0.01106994787452712</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0.0009638351215188474</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>0.004260056751199901</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>0.0107196465601912</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>0.001714354981946688</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>1.256438897757982e-10</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>9.324736549418949e-11</v>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>0.005121796925822195</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>-0.51151695790439</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>0.04543535145661821</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>-0.1429511322129842</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>-0.2105190978883724</v>
-      </c>
-      <c r="O2" s="3" t="n">
-        <v>0.04759920921230281</v>
-      </c>
-      <c r="P2" s="3" t="n">
-        <v>0.1131717505081041</v>
-      </c>
-      <c r="Q2" s="3" t="n">
-        <v>-0.006948132450303703</v>
-      </c>
-      <c r="R2" s="3" t="n">
-        <v>0.1705487444437477</v>
-      </c>
-      <c r="S2" s="3" t="n">
-        <v>0.1426130105838598</v>
-      </c>
-      <c r="T2" s="3" t="n">
-        <v>0.1121617489438894</v>
-      </c>
-      <c r="U2" s="3" t="n">
-        <v>0.09722115133313633</v>
-      </c>
-      <c r="V2" s="3" t="n">
-        <v>0.110456455058216</v>
-      </c>
-      <c r="W2" s="3" t="n">
-        <v>0.1051124257000614</v>
-      </c>
-      <c r="X2" s="3" t="n">
-        <v>0.1198055228101544</v>
-      </c>
-      <c r="Y2" s="3" t="n">
-        <v>0.1420809411269349</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="3" s="4">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="B3" s="3" t="n">
+        <v>0.1385909283782561</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0.01050664818474728</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0.001176417984417368</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.004759879099648455</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.009496628304978187</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0.001849711840304627</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>1.127368128607484e-10</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>8.768050621303033e-11</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0.006256578361578916</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>-0.483545571782841</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0.04256289451534556</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>-0.1676105457660406</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>-0.2060824955672104</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>0.04853126607488272</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>0.1057432012904757</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>-0.00447976343857507</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>0.1651425896038074</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>0.1465595186880449</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>0.1272481894178498</v>
+      </c>
+      <c r="U3" s="3" t="n">
+        <v>0.1078130448519441</v>
+      </c>
+      <c r="V3" s="3" t="n">
+        <v>0.102646633060844</v>
+      </c>
+      <c r="W3" s="3" t="n">
+        <v>0.1093472911632663</v>
+      </c>
+      <c r="X3" s="3" t="n">
+        <v>0.107830896961512</v>
+      </c>
+      <c r="Y3" s="3" t="n">
+        <v>0.1334118362527315</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>TSLA</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>0.1509377355213447</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>0.04829205583879663</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>0.003967244396418783</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>0.01453355824323124</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>0.02485114489758947</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>0.005434399282194052</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>7.352085461773991e-10</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>5.273594266517581e-10</v>
-      </c>
-      <c r="J3" s="3" t="n">
-        <v>0.009517786550298521</v>
-      </c>
-      <c r="K3" s="3" t="n">
-        <v>-2.349112636860576</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>0.1521597684603392</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>-0.5516617738005419</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>-0.2967455595863266</v>
-      </c>
-      <c r="O3" s="3" t="n">
-        <v>0.161472894255981</v>
-      </c>
-      <c r="P3" s="3" t="n">
-        <v>-0.2022485898745222</v>
-      </c>
-      <c r="Q3" s="3" t="n">
-        <v>-0.4317383272461738</v>
-      </c>
-      <c r="R3" s="3" t="n">
-        <v>0.2355375191423913</v>
-      </c>
-      <c r="S3" s="3" t="n">
-        <v>0.1339113691802713</v>
-      </c>
-      <c r="T3" s="3" t="n">
-        <v>0.1126646699860898</v>
-      </c>
-      <c r="U3" s="3" t="n">
-        <v>0.08611165322652134</v>
-      </c>
-      <c r="V3" s="3" t="n">
-        <v>0.06256545940181563</v>
-      </c>
-      <c r="W3" s="3" t="n">
-        <v>0.08695590222156396</v>
-      </c>
-      <c r="X3" s="3" t="n">
-        <v>0.1431282108576752</v>
-      </c>
-      <c r="Y3" s="3" t="n">
-        <v>0.1391252159836715</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="4" s="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="B4" s="3" t="n">
+        <v>0.1501123784387246</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.04612699993502843</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.004452833277145399</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.01655896306969518</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.02196792746131501</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>0.005992214192937989</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>7.583055445389367e-10</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>5.432902149686715e-10</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.01501284839232625</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>-2.230352892383939</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0.1585061151949421</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>-0.6529687690722783</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>-0.2921015150100861</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>0.1659283397268095</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>-0.2082966909096421</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>-0.443708215485173</v>
+      </c>
+      <c r="R4" s="3" t="n">
+        <v>0.225364770843834</v>
+      </c>
+      <c r="S4" s="3" t="n">
+        <v>0.1381882030621805</v>
+      </c>
+      <c r="T4" s="3" t="n">
+        <v>0.1172233139627159</v>
+      </c>
+      <c r="U4" s="3" t="n">
+        <v>0.09296147935881117</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>0.05748897378551517</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>0.09152875398670732</v>
+      </c>
+      <c r="X4" s="3" t="n">
+        <v>0.1405952647913003</v>
+      </c>
+      <c r="Y4" s="3" t="n">
+        <v>0.1366492402089356</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>PLUG</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>0.139737681297814</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>0.08771038850914158</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0.006456843100750385</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0.0218109082869842</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>0.07006959456924344</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>0.009979574230356839</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>1.441592935345299e-10</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>7.519938481449504e-11</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>-0.006868826760564582</v>
-      </c>
-      <c r="K4" s="3" t="n">
-        <v>-4.280086590864762</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>0.02546828206027066</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>-1.007542051032072</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>-1.487825978478411</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>0.03806583469283134</v>
-      </c>
-      <c r="P4" s="3" t="n">
-        <v>-0.02267335264380377</v>
-      </c>
-      <c r="Q4" s="3" t="n">
-        <v>-0.05244860975406021</v>
-      </c>
-      <c r="R4" s="3" t="n">
-        <v>0.4165813462087934</v>
-      </c>
-      <c r="S4" s="3" t="n">
-        <v>0.1523224364820338</v>
-      </c>
-      <c r="T4" s="3" t="n">
-        <v>0.1305075871960828</v>
-      </c>
-      <c r="U4" s="3" t="n">
-        <v>0.08627099045866167</v>
-      </c>
-      <c r="V4" s="3" t="n">
-        <v>0.09721422086977258</v>
-      </c>
-      <c r="W4" s="3" t="n">
-        <v>0.1082798098612328</v>
-      </c>
-      <c r="X4" s="3" t="n">
-        <v>0.002353776623413573</v>
-      </c>
-      <c r="Y4" s="3" t="n">
-        <v>0.006469832300009352</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="5" s="4">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="B5" s="3" t="n">
+        <v>0.137114581169123</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.08166580030685124</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.007217073132578467</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.0249984170025428</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0.04954374236238585</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0.0106921106147825</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>1.586549400427411e-10</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>7.741208127169423e-11</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>-0.008958351860397921</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>-3.981024836687937</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0.02747215132586744</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>-1.150648239630023</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>-1.223808236677121</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>0.04442122561322988</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>-0.02229436639244444</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>-0.05326259367670187</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>0.4015410144813033</v>
+      </c>
+      <c r="S5" s="3" t="n">
+        <v>0.1607060218261482</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>0.1397617031435922</v>
+      </c>
+      <c r="U5" s="3" t="n">
+        <v>0.09717623500396873</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <v>0.07650906078671398</v>
+      </c>
+      <c r="W5" s="3" t="n">
+        <v>0.1151797229826008</v>
+      </c>
+      <c r="X5" s="3" t="n">
+        <v>0.002569980053887135</v>
+      </c>
+      <c r="Y5" s="3" t="n">
+        <v>0.006556261721785637</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>NKLA</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>0.1400185252141773</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>0.02410674020589887</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0.001895446801812674</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>0.004439470328535895</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>0.01648532172998477</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>0.003570646128387971</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>6.191425479028914e-09</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>2.674109862407788e-10</v>
-      </c>
-      <c r="J5" s="3" t="n">
-        <v>-0.003629460444900821</v>
-      </c>
-      <c r="K5" s="3" t="n">
-        <v>-1.34219716588954</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>-0.07312480113109572</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>-0.2118434947924622</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>-0.4047399872541825</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>-0.06314359019593282</v>
-      </c>
-      <c r="P5" s="3" t="n">
-        <v>0.05554449371410183</v>
-      </c>
-      <c r="Q5" s="3" t="n">
-        <v>-0.0009912682447493603</v>
-      </c>
-      <c r="R5" s="3" t="n">
-        <v>0.2249774323845742</v>
-      </c>
-      <c r="S5" s="3" t="n">
-        <v>0.1642175746493672</v>
-      </c>
-      <c r="T5" s="3" t="n">
-        <v>0.1437189204751534</v>
-      </c>
-      <c r="U5" s="3" t="n">
-        <v>0.07490929489843506</v>
-      </c>
-      <c r="V5" s="3" t="n">
-        <v>0.128737288204179</v>
-      </c>
-      <c r="W5" s="3" t="n">
-        <v>0.1239254875859819</v>
-      </c>
-      <c r="X5" s="3" t="n">
-        <v>0.1225350439862598</v>
-      </c>
-      <c r="Y5" s="3" t="n">
-        <v>0.01697895781604921</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="6" s="4">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="B6" s="3" t="n">
+        <v>0.1367167143397206</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.02314229710689453</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.002204323359715545</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0.005159682028524805</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0.01701290855751802</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>0.004072116730582306</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>5.884292817423834e-09</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>2.531021603109672e-10</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>-0.00394161897945279</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>-1.287373995580736</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>-0.06874997834314774</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>-0.250303064702823</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>-0.4513940847565958</v>
+      </c>
+      <c r="O6" s="3" t="n">
+        <v>-0.06085719663435713</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>0.05406108151807273</v>
+      </c>
+      <c r="Q6" s="3" t="n">
+        <v>-0.001910059861398935</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>0.2054564861933204</v>
+      </c>
+      <c r="S6" s="3" t="n">
+        <v>0.1667226846709638</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>0.1507470459073334</v>
+      </c>
+      <c r="U6" s="3" t="n">
+        <v>0.08168630253695956</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <v>0.1345216979067013</v>
+      </c>
+      <c r="W6" s="3" t="n">
+        <v>0.1330197731249609</v>
+      </c>
+      <c r="X6" s="3" t="n">
+        <v>0.1127224085050003</v>
+      </c>
+      <c r="Y6" s="3" t="n">
+        <v>0.01512360115476023</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>MSFT</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>0.1377744771738686</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>0.01077240239978401</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0.0009791177603384398</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>0.003490125726474338</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>0.001241682024925196</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>0.001353478261000405</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>5.019250107072721e-12</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>3.415416791997129e-11</v>
-      </c>
-      <c r="J6" s="3" t="n">
-        <v>0.001396272769249888</v>
-      </c>
-      <c r="K6" s="3" t="n">
-        <v>-0.5338320807505512</v>
-      </c>
-      <c r="L6" s="3" t="n">
-        <v>0.01644695307840659</v>
-      </c>
-      <c r="M6" s="3" t="n">
-        <v>-0.1493885131128801</v>
-      </c>
-      <c r="N6" s="3" t="n">
-        <v>0.009715207703908966</v>
-      </c>
-      <c r="O6" s="3" t="n">
-        <v>0.01818046430218447</v>
-      </c>
-      <c r="P6" s="3" t="n">
-        <v>0.05790247896986352</v>
-      </c>
-      <c r="Q6" s="3" t="n">
-        <v>0.06462436139213427</v>
-      </c>
-      <c r="R6" s="3" t="n">
-        <v>0.2405660260351586</v>
-      </c>
-      <c r="S6" s="3" t="n">
-        <v>0.1871916114080155</v>
-      </c>
-      <c r="T6" s="3" t="n">
-        <v>0.1910250343757978</v>
-      </c>
-      <c r="U6" s="3" t="n">
-        <v>0.1439554320597602</v>
-      </c>
-      <c r="V6" s="3" t="n">
-        <v>0.01689881577335669</v>
-      </c>
-      <c r="W6" s="3" t="n">
-        <v>0.1505446695753559</v>
-      </c>
-      <c r="X6" s="3" t="n">
-        <v>0.01928539008151347</v>
-      </c>
-      <c r="Y6" s="3" t="n">
-        <v>0.0505330206910418</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="7" s="4">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>SNE</t>
-        </is>
-      </c>
       <c r="B7" s="3" t="n">
-        <v>0.1390518612329022</v>
+        <v>0.1345400174778676</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.0147110386237944</v>
+        <v>0.01036200100409962</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.00138782395704841</v>
+        <v>0.001119259071693009</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.004734652117552338</v>
+        <v>0.003971722791948849</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>-0.0002874154348478644</v>
+        <v>0.0006543173600419557</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>0.001912574355548698</v>
+        <v>0.001466221734135586</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>2.350205226318901e-10</v>
+        <v>5.019653753372684e-12</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1.075817603716296e-09</v>
+        <v>3.353349052686357e-11</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>6.863564669539238e-05</v>
+        <v>0.002384517343013836</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>-0.742963482844535</v>
+        <v>-0.5127426748859708</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>-0.003199212426994573</v>
+        <v>0.01702644247593209</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>-0.239139985282929</v>
+        <v>-0.1745143201006574</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>0.00665817495652387</v>
+        <v>0.02079050501177461</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>-0.002394210688817426</v>
+        <v>0.01951049090438907</v>
       </c>
       <c r="P7" s="3" t="n">
-        <v>-0.04093712871211268</v>
+        <v>0.05828798079919199</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>-0.0318620221990337</v>
+        <v>0.06447206528427187</v>
       </c>
       <c r="R7" s="3" t="n">
-        <v>0.2076813235129483</v>
+        <v>0.2208767591637097</v>
       </c>
       <c r="S7" s="3" t="n">
-        <v>0.2013858357184395</v>
+        <v>0.1953307709446786</v>
       </c>
       <c r="T7" s="3" t="n">
-        <v>0.1932597662311594</v>
+        <v>0.201067128291379</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>0.1446719473921602</v>
+        <v>0.1539560436556384</v>
       </c>
       <c r="V7" s="3" t="n">
-        <v>-0.002803713685289555</v>
+        <v>0.009620442903557196</v>
       </c>
       <c r="W7" s="3" t="n">
-        <v>0.1541645847455442</v>
+        <v>0.154354047161639</v>
       </c>
       <c r="X7" s="3" t="n">
-        <v>0.04094329995539177</v>
+        <v>0.01815311472078176</v>
       </c>
       <c r="Y7" s="3" t="n">
-        <v>0.06069695612964611</v>
+        <v>0.04664169315861624</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>SNE</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0.138828402702272</v>
+        <v>0.1362359037010507</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0.02368181615127902</v>
+        <v>0.01429507612645025</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.00211017440843641</v>
+        <v>0.001575430175363643</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.007552945430953245</v>
+        <v>0.005439131765689395</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>-0.002899019173317308</v>
+        <v>0.0004191584755106373</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>0.002895210326201101</v>
+        <v>0.002068530526622674</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>1.906383891769283e-11</v>
+        <v>2.348807752275892e-10</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>1.489053133537491e-10</v>
+        <v>1.078206231965275e-09</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>-0.0001074738018242117</v>
+        <v>0.0001337265080490603</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>-1.205251220264326</v>
+        <v>-0.7216613100202224</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>-0.009209855488292496</v>
+        <v>-0.001553549086587638</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>-0.3832348513798011</v>
+        <v>-0.2746776158112832</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>0.06984299877061122</v>
+        <v>-0.006554733305411077</v>
       </c>
       <c r="O8" s="3" t="n">
-        <v>-0.01256293094118213</v>
+        <v>-0.0009471621737110984</v>
       </c>
       <c r="P8" s="3" t="n">
-        <v>0.007938924468274124</v>
+        <v>-0.04028419930669253</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>-0.008293455278021436</v>
+        <v>-0.03136447011002497</v>
       </c>
       <c r="R8" s="3" t="n">
-        <v>0.2047027475138697</v>
+        <v>0.1883611222308824</v>
       </c>
       <c r="S8" s="3" t="n">
-        <v>0.2258712225773657</v>
+        <v>0.2058170513959711</v>
       </c>
       <c r="T8" s="3" t="n">
-        <v>0.2245530239219594</v>
+        <v>0.1986039076849226</v>
       </c>
       <c r="U8" s="3" t="n">
-        <v>0.1672249785490406</v>
+        <v>0.1534964713851671</v>
       </c>
       <c r="V8" s="3" t="n">
-        <v>-0.02037186230044567</v>
+        <v>0.004278437920373342</v>
       </c>
       <c r="W8" s="3" t="n">
-        <v>0.1734779448849674</v>
+        <v>0.155307547608612</v>
       </c>
       <c r="X8" s="3" t="n">
-        <v>0.005001859988906268</v>
+        <v>0.03783677720947085</v>
       </c>
       <c r="Y8" s="3" t="n">
-        <v>0.01954008486433653</v>
+        <v>0.05629868456460045</v>
       </c>
     </row>
   </sheetData>
@@ -1180,12 +1181,12 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="3" width="11.52"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="12.8" r="1" s="3">
+    <row customHeight="1" ht="12.8" r="1" s="4">
       <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Stock</t>
@@ -1335,16 +1336,16 @@
   </sheetPr>
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K2" activeCellId="0" pane="topLeft" sqref="K2"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="3" width="11.52"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="12.8" r="1" s="3">
+    <row customHeight="1" ht="12.8" r="1" s="4">
       <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Stock</t>
@@ -1471,86 +1472,86 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row customHeight="1" ht="12.8" r="2" s="4">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>SNE</t>
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>0.1365796825417144</v>
+        <v>0.136579682541714</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.002216147574899179</v>
+        <v>0.00221614757489918</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.0001571081234681272</v>
+        <v>0.000157108123468127</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.0006223061673251691</v>
+        <v>0.000622306167325169</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>5.016956732221472e-05</v>
+        <v>5.01695673222147e-05</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>0.0002070734884176489</v>
+        <v>0.000207073488417649</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>-1.212572110247775e-09</v>
+        <v>-1.21257211024778e-09</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>-8.384574341712387e-10</v>
+        <v>-8.38457434171239e-10</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>0.0003007498013556107</v>
+        <v>0.000300749801355611</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>-0.1107768565389296</v>
+        <v>-0.11077685653893</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>0.0008776326303478116</v>
+        <v>0.000877632630347812</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>-0.03034584438311547</v>
+        <v>-0.0303458443831155</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>0.001180566301894219</v>
+        <v>0.00118056630189422</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>0.001196233101307122</v>
+        <v>0.00119623310130712</v>
       </c>
       <c r="P2" s="3" t="n">
-        <v>0.001750068167384502</v>
+        <v>0.0017500681673845</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>0.001543948786416403</v>
+        <v>0.0015439487864164</v>
       </c>
       <c r="R2" s="3" t="n">
-        <v>0.5919332697401547</v>
+        <v>0.591933269740155</v>
       </c>
       <c r="S2" s="3" t="n">
-        <v>0.008050913322968934</v>
+        <v>0.00805091332296894</v>
       </c>
       <c r="T2" s="3" t="n">
-        <v>0.0007966004985989171</v>
+        <v>0.000796600498598917</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>0.004903962132844019</v>
+        <v>0.00490396213284402</v>
       </c>
       <c r="V2" s="3" t="n">
-        <v>0.3921716076272256</v>
+        <v>0.392171607627226</v>
       </c>
       <c r="W2" s="3" t="n">
-        <v>0.002160094560687294</v>
+        <v>0.00216009456068729</v>
       </c>
       <c r="X2" s="3" t="n">
-        <v>-1.073399045456651e-05</v>
+        <v>-1.07339904545665e-05</v>
       </c>
       <c r="Y2" s="3" t="n">
-        <v>-5.713892024917514e-06</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>-5.71389202491751e-06</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="4">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>NIO</t>
@@ -1560,76 +1561,76 @@
         <v>0.140390802789484</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.003301686603421307</v>
+        <v>0.00330168660342131</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.0002480525417674323</v>
+        <v>0.000248052541767432</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.0009357037951675747</v>
+        <v>0.000935703795167575</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>-0.0004825428076010712</v>
+        <v>-0.000482542807601071</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>0.0004057437854160523</v>
+        <v>0.000405743785416052</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>1.669580024808732e-10</v>
+        <v>1.66958002480873e-10</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.699041320721213e-10</v>
+        <v>1.69904132072121e-10</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>-5.350486214309017e-05</v>
+        <v>-5.35048621430902e-05</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>-0.1668236787220054</v>
+        <v>-0.166823678722005</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>-0.001417060603973989</v>
+        <v>-0.00141706060397399</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>-0.04963762027727043</v>
+        <v>-0.0496376202772704</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>0.008389363929595191</v>
+        <v>0.008389363929595189</v>
       </c>
       <c r="O3" s="3" t="n">
         <v>-0.00152330597909392</v>
       </c>
       <c r="P3" s="3" t="n">
-        <v>-0.001455672401689893</v>
+        <v>-0.00145567240168989</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>0.001770431029081104</v>
+        <v>0.0017704310290811</v>
       </c>
       <c r="R3" s="3" t="n">
-        <v>1.137462851636135</v>
+        <v>1.13746285163614</v>
       </c>
       <c r="S3" s="3" t="n">
-        <v>0.02357114397100765</v>
+        <v>0.0235711439710077</v>
       </c>
       <c r="T3" s="3" t="n">
-        <v>0.002491005582330114</v>
+        <v>0.00249100558233011</v>
       </c>
       <c r="U3" s="3" t="n">
-        <v>0.01624218186127702</v>
+        <v>0.016242181861277</v>
       </c>
       <c r="V3" s="3" t="n">
-        <v>-0.1861628357190317</v>
+        <v>-0.186162835719032</v>
       </c>
       <c r="W3" s="3" t="n">
-        <v>0.006395562941332923</v>
+        <v>0.00639556294133292</v>
       </c>
       <c r="X3" s="3" t="n">
-        <v>5.285051982544759e-08</v>
+        <v>5.28505198254476e-08</v>
       </c>
       <c r="Y3" s="3" t="n">
-        <v>3.687642942126135e-08</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>3.68764294212614e-08</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="4" s="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>RIDE</t>
@@ -1639,46 +1640,46 @@
         <v>0.138058774745679</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.002236427120183643</v>
+        <v>0.00223642712018364</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.0001516328183570822</v>
+        <v>0.000151632818357082</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.0005318391824838172</v>
+        <v>0.000531839182483817</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>-0.0002792598280523559</v>
+        <v>-0.000279259828052356</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>0.0002263791170622916</v>
+        <v>0.000226379117062292</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>-1.247785080755039e-09</v>
+        <v>-1.24778508075504e-09</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>-6.784216718761849e-10</v>
+        <v>-6.78421671876185e-10</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>-1.024057670902861e-05</v>
+        <v>-1.02405767090286e-05</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>-0.1125574213158327</v>
+        <v>-0.112557421315833</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>-0.001240203772218537</v>
+        <v>-0.00124020377221854</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>-0.02783304235846106</v>
+        <v>-0.0278330423584611</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>0.004190813667525487</v>
+        <v>0.00419081366752549</v>
       </c>
       <c r="O4" s="3" t="n">
         <v>-0.00120550048682852</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>-0.004000942645409489</v>
+        <v>-0.00400094264540949</v>
       </c>
       <c r="Q4" s="3" t="n">
         <v>-0.00624770682789231</v>
@@ -1687,490 +1688,490 @@
         <v>1.09321731953475</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>0.01400961560426633</v>
+        <v>0.0140096156042663</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>0.001188507625188342</v>
+        <v>0.00118850762518834</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>0.008112684397376165</v>
+        <v>0.00811268439737617</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>-0.1198645365802747</v>
+        <v>-0.119864536580275</v>
       </c>
       <c r="W4" s="3" t="n">
-        <v>0.003338389618487537</v>
+        <v>0.00333838961848754</v>
       </c>
       <c r="X4" s="3" t="n">
-        <v>-1.634858646817933e-06</v>
+        <v>-1.63485864681793e-06</v>
       </c>
       <c r="Y4" s="3" t="n">
-        <v>-3.453411471495647e-07</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>-3.45341147149565e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="5" s="4">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>FUV</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.1339329788895788</v>
+        <v>0.133932978889579</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>0.00204546003815904</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.0001400641191862473</v>
+        <v>0.000140064119186247</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.0004940213023491799</v>
+        <v>0.00049402130234918</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>0.0003338168727394537</v>
+        <v>0.000333816872739454</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>0.0001956874586839811</v>
+        <v>0.000195687458683981</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>6.517667980300445e-09</v>
+        <v>6.51766798030045e-09</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>2.755400861872415e-09</v>
+        <v>2.75540086187241e-09</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>0.0002635937347331295</v>
+        <v>0.000263593734733129</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>-0.1032038728865534</v>
+        <v>-0.103203872886553</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>-0.0004015089297842753</v>
+        <v>-0.000401508929784275</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>-0.02423859184948885</v>
+        <v>-0.0242385918494888</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>-0.005478908273386606</v>
+        <v>-0.00547890827338661</v>
       </c>
       <c r="O5" s="3" t="n">
-        <v>-7.624335085964149e-05</v>
+        <v>-7.624335085964151e-05</v>
       </c>
       <c r="P5" s="3" t="n">
-        <v>0.006692330220695156</v>
+        <v>0.00669233022069516</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>0.002479197308736005</v>
+        <v>0.00247919730873601</v>
       </c>
       <c r="R5" s="3" t="n">
-        <v>0.9202840371170461</v>
+        <v>0.920284037117046</v>
       </c>
       <c r="S5" s="3" t="n">
         <v>0.00942445546988136</v>
       </c>
       <c r="T5" s="3" t="n">
-        <v>0.0007226563714846885</v>
+        <v>0.000722656371484688</v>
       </c>
       <c r="U5" s="3" t="n">
-        <v>0.004728718291694773</v>
+        <v>0.00472871829169477</v>
       </c>
       <c r="V5" s="3" t="n">
         <v>0.0629427015028059</v>
       </c>
       <c r="W5" s="3" t="n">
-        <v>0.001894083386032896</v>
+        <v>0.0018940833860329</v>
       </c>
       <c r="X5" s="3" t="n">
-        <v>2.123017876318995e-06</v>
+        <v>2.12301787631899e-06</v>
       </c>
       <c r="Y5" s="3" t="n">
-        <v>1.224843177832577e-06</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1.22484317783258e-06</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="6" s="4">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>FCEL</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>0.1388322785493898</v>
+        <v>0.13883227854939</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>0.001207248165282745</v>
+        <v>0.00120724816528275</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>8.452156315099475e-05</v>
+        <v>8.45215631509948e-05</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.0002826090666700295</v>
+        <v>0.000282609066670029</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>-0.0001434427553182709</v>
+        <v>-0.000143442755318271</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>0.0001171634215140675</v>
+        <v>0.000117163421514068</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>6.862591276097072e-11</v>
+        <v>6.86259127609707e-11</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>1.147042855419848e-11</v>
+        <v>1.14704285541985e-11</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1.571140499557461e-05</v>
+        <v>1.57114049955746e-05</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>-0.06111211688192297</v>
+        <v>-0.061112116881923</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>-0.0002498232601020551</v>
+        <v>-0.000249823260102055</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>-0.01439744604388904</v>
+        <v>-0.014397446043889</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>0.003465253133698189</v>
+        <v>0.00346525313369819</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>-0.0001380411328568036</v>
+        <v>-0.000138041132856804</v>
       </c>
       <c r="P6" s="3" t="n">
-        <v>0.001467484937465771</v>
+        <v>0.00146748493746577</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>0.0008690481970982136</v>
+        <v>0.000869048197098214</v>
       </c>
       <c r="R6" s="3" t="n">
-        <v>1.068975458460943</v>
+        <v>1.06897545846094</v>
       </c>
       <c r="S6" s="3" t="n">
-        <v>0.007904132835825906</v>
+        <v>0.00790413283582591</v>
       </c>
       <c r="T6" s="3" t="n">
-        <v>0.0007279231062828069</v>
+        <v>0.000727923106282807</v>
       </c>
       <c r="U6" s="3" t="n">
-        <v>0.005012299812382395</v>
+        <v>0.0050122998123824</v>
       </c>
       <c r="V6" s="3" t="n">
-        <v>-0.08459481436091178</v>
+        <v>-0.0845948143609118</v>
       </c>
       <c r="W6" s="3" t="n">
-        <v>0.001974772009455681</v>
+        <v>0.00197477200945568</v>
       </c>
       <c r="X6" s="3" t="n">
-        <v>3.022912175851156e-08</v>
+        <v>3.02291217585116e-08</v>
       </c>
       <c r="Y6" s="3" t="n">
-        <v>1.979068996718308e-07</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1.97906899671831e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="7" s="4">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>CBAT</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.1373898935269345</v>
+        <v>0.137389893526935</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.001000505150975067</v>
+        <v>0.00100050515097507</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>7.083356666853193e-05</v>
+        <v>7.08335666685319e-05</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.0002187206642030935</v>
+        <v>0.000218720664203093</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>7.308223406688899e-05</v>
+        <v>7.3082234066889e-05</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>9.885917414383504e-05</v>
+        <v>9.8859174143835e-05</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>1.832454305661435e-10</v>
+        <v>1.83245430566143e-10</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1.513989915917859e-10</v>
+        <v>1.51398991591786e-10</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>-9.317499031815299e-05</v>
+        <v>-9.3174990318153e-05</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>-0.04965203276413535</v>
+        <v>-0.0496520327641354</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>-0.0001719820301421706</v>
+        <v>-0.000171982030142171</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>-0.01120360223681758</v>
+        <v>-0.0112036022368176</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>-0.002294425496864808</v>
+        <v>-0.00229442549686481</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>-0.0002419721460811934</v>
+        <v>-0.000241972146081193</v>
       </c>
       <c r="P7" s="3" t="n">
-        <v>-0.0003882421322900391</v>
+        <v>-0.000388242132290039</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>-0.0001701073950547276</v>
+        <v>-0.000170107395054728</v>
       </c>
       <c r="R7" s="3" t="n">
-        <v>0.9115968398569188</v>
+        <v>0.911596839856919</v>
       </c>
       <c r="S7" s="3" t="n">
-        <v>0.005545060216527983</v>
+        <v>0.00554506021652798</v>
       </c>
       <c r="T7" s="3" t="n">
         <v>0.000490912219442732</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>0.003500044752658145</v>
+        <v>0.00350004475265814</v>
       </c>
       <c r="V7" s="3" t="n">
-        <v>0.07750122271313249</v>
+        <v>0.07750122271313251</v>
       </c>
       <c r="W7" s="3" t="n">
         <v>0.00136523209104068</v>
       </c>
       <c r="X7" s="3" t="n">
-        <v>4.488520922262697e-07</v>
+        <v>4.4885209222627e-07</v>
       </c>
       <c r="Y7" s="3" t="n">
-        <v>2.392981870175791e-07</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>2.39298187017579e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="8" s="4">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>BLNK</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0.1396342843251271</v>
+        <v>0.139634284325127</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0.004639776084325538</v>
+        <v>0.00463977608432554</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.0003258124075229741</v>
+        <v>0.000325812407522974</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.001166057581280599</v>
+        <v>0.0011660575812806</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.001061666730149971</v>
+        <v>0.00106166673014997</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>0.0005050567141821847</v>
+        <v>0.000505056714182185</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>1.361917264801037e-09</v>
+        <v>1.36191726480104e-09</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>1.222425414346388e-09</v>
+        <v>1.22242541434639e-09</v>
       </c>
       <c r="J8" s="3" t="n">
         <v>9.23309107013092e-05</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>-0.2310246233996237</v>
+        <v>-0.231024623399624</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>0.005013629626670239</v>
+        <v>0.00501362962667024</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>-0.05122257272395421</v>
+        <v>-0.0512225727239542</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>-0.01363268924532307</v>
+        <v>-0.0136326892453231</v>
       </c>
       <c r="O8" s="3" t="n">
-        <v>0.006038206553258089</v>
+        <v>0.00603820655325809</v>
       </c>
       <c r="P8" s="3" t="n">
-        <v>0.004045045748874083</v>
+        <v>0.00404504574887408</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>0.002725961832294195</v>
+        <v>0.0027259618322942</v>
       </c>
       <c r="R8" s="3" t="n">
         <v>0.818418639811601</v>
       </c>
       <c r="S8" s="3" t="n">
-        <v>0.02266311261136788</v>
+        <v>0.0226631126113679</v>
       </c>
       <c r="T8" s="3" t="n">
-        <v>0.002238022847463316</v>
+        <v>0.00223802284746332</v>
       </c>
       <c r="U8" s="3" t="n">
         <v>0.0137190155983109</v>
       </c>
       <c r="V8" s="3" t="n">
-        <v>0.1373739425332199</v>
+        <v>0.13737394253322</v>
       </c>
       <c r="W8" s="3" t="n">
         <v>0.00558695396037438</v>
       </c>
       <c r="X8" s="3" t="n">
-        <v>1.780917098829098e-07</v>
+        <v>1.7809170988291e-07</v>
       </c>
       <c r="Y8" s="3" t="n">
-        <v>1.345459526431084e-07</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1.34545952643108e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="9" s="4">
       <c r="A9" s="3" t="inlineStr">
         <is>
           <t>TSLA</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>0.1386507903716349</v>
+        <v>0.138650790371635</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>0.03152219335915932</v>
+        <v>0.0315221933591593</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.002500150192751971</v>
+        <v>0.00250015019275197</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.008599544053265684</v>
+        <v>0.008599544053265681</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>-0.003756259701969515</v>
+        <v>-0.00375625970196951</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>0.003810400885647823</v>
+        <v>0.00381040088564782</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>3.752675972548288e-10</v>
+        <v>3.75267597254829e-10</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>4.819069815380915e-10</v>
+        <v>4.81906981538092e-10</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>0.0001366628207377142</v>
+        <v>0.000136662820737714</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>-1.599042466700336</v>
+        <v>-1.59904246670034</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>0.01483166486904013</v>
+        <v>0.0148316648690401</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>-0.4090898780750495</v>
+        <v>-0.409089878075049</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>0.1010466566265678</v>
+        <v>0.101046656626568</v>
       </c>
       <c r="O9" s="3" t="n">
-        <v>0.01312366030283914</v>
+        <v>0.0131236603028391</v>
       </c>
       <c r="P9" s="3" t="n">
-        <v>0.008189822173629784</v>
+        <v>0.00818982217362979</v>
       </c>
       <c r="Q9" s="3" t="n">
-        <v>0.01012660496456165</v>
+        <v>0.0101266049645617</v>
       </c>
       <c r="R9" s="3" t="n">
-        <v>-2.843852370715392</v>
+        <v>-2.84385237071539</v>
       </c>
       <c r="S9" s="3" t="n">
-        <v>-0.5278654752995863</v>
+        <v>-0.5278654752995861</v>
       </c>
       <c r="T9" s="3" t="n">
-        <v>-0.05150882219860459</v>
+        <v>-0.0515088221986046</v>
       </c>
       <c r="U9" s="3" t="n">
-        <v>-0.3710935068659833</v>
+        <v>-0.371093506865983</v>
       </c>
       <c r="V9" s="3" t="n">
         <v>4.94358372389054</v>
       </c>
       <c r="W9" s="3" t="n">
-        <v>-0.1492483940277798</v>
+        <v>-0.14924839402778</v>
       </c>
       <c r="X9" s="3" t="n">
-        <v>-7.692584579724937e-06</v>
+        <v>-7.692584579724941e-06</v>
       </c>
       <c r="Y9" s="3" t="n">
-        <v>-7.462198613545672e-06</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>-7.46219861354567e-06</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="10" s="4">
       <c r="A10" s="3" t="inlineStr">
         <is>
           <t>AMZN</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>0.1383523795847323</v>
+        <v>0.138352379584732</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0.06698570990662917</v>
+        <v>0.06698570990662921</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.005338954389505024</v>
+        <v>0.00533895438950502</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0.01814090880617904</v>
+        <v>0.018140908806179</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0.001320684761528799</v>
+        <v>0.0013206847615288</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>0.008129214262400325</v>
+        <v>0.00812921426240033</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>5.220612349965496e-08</v>
+        <v>5.2206123499655e-08</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>8.206121174640703e-08</v>
+        <v>8.2061211746407e-08</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>0.002716943231144022</v>
+        <v>0.00271694323114402</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>-3.356220903856804</v>
+        <v>-3.3562209038568</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0.003021727325451415</v>
+        <v>0.00302172732545141</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>-0.9422960039886694</v>
+        <v>-0.942296003988669</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>-0.02865703110885632</v>
+        <v>-0.0286570311088563</v>
       </c>
       <c r="O10" s="3" t="n">
-        <v>0.008806618893731752</v>
+        <v>0.00880661889373175</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>-0.02559068320726264</v>
+        <v>-0.0255906832072626</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>0.02575127394472895</v>
+        <v>0.025751273944729</v>
       </c>
       <c r="R10" s="3" t="n">
-        <v>0.03510849234028039</v>
+        <v>0.0351084923402804</v>
       </c>
       <c r="S10" s="3" t="n">
-        <v>0.01292777291283585</v>
+        <v>0.0129277729128359</v>
       </c>
       <c r="T10" s="3" t="n">
-        <v>0.001162750983675746</v>
+        <v>0.00116275098367575</v>
       </c>
       <c r="U10" s="3" t="n">
-        <v>0.007625953832607388</v>
+        <v>0.00762595383260739</v>
       </c>
       <c r="V10" s="3" t="n">
-        <v>0.9401090440092906</v>
+        <v>0.940109044009291</v>
       </c>
       <c r="W10" s="3" t="n">
         <v>0.00306006342908693</v>
@@ -2179,102 +2180,102 @@
         <v>4.45429767334308e-06</v>
       </c>
       <c r="Y10" s="3" t="n">
-        <v>1.468194549674892e-06</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1.46819454967489e-06</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="11" s="4">
       <c r="A11" s="3" t="inlineStr">
         <is>
           <t>AAPL</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>0.1388844859697914</v>
+        <v>0.138884485969791</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0.003006998190787461</v>
+        <v>0.00300699819078746</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.0002127092263237959</v>
+        <v>0.000212709226323796</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0.0007839183979900401</v>
+        <v>0.00078391839799004</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0.0001407127057428467</v>
+        <v>0.000140712705742847</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>0.0003171818137868449</v>
+        <v>0.000317181813786845</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>-1.749450642433621e-11</v>
+        <v>-1.74945064243362e-11</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>9.137919544518223e-11</v>
+        <v>9.13791954451822e-11</v>
       </c>
       <c r="J11" s="3" t="n">
         <v>2.90600455511205e-05</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>-0.1511972228940781</v>
+        <v>-0.151197222894078</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>0.002671338898856779</v>
+        <v>0.00267133889885678</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>-0.03645114795390803</v>
+        <v>-0.036451147953908</v>
       </c>
       <c r="N11" s="3" t="n">
-        <v>0.001422776808864739</v>
+        <v>0.00142277680886474</v>
       </c>
       <c r="O11" s="3" t="n">
-        <v>0.002646139524095204</v>
+        <v>0.0026461395240952</v>
       </c>
       <c r="P11" s="3" t="n">
-        <v>0.005454280840753256</v>
+        <v>0.00545428084075326</v>
       </c>
       <c r="Q11" s="3" t="n">
-        <v>0.0005002561642402024</v>
+        <v>0.000500256164240202</v>
       </c>
       <c r="R11" s="3" t="n">
-        <v>0.6643086251633646</v>
+        <v>0.664308625163365</v>
       </c>
       <c r="S11" s="3" t="n">
-        <v>0.01143058494887313</v>
+        <v>0.0114305849488731</v>
       </c>
       <c r="T11" s="3" t="n">
-        <v>0.001082677065070497</v>
+        <v>0.0010826770650705</v>
       </c>
       <c r="U11" s="3" t="n">
-        <v>0.007060551052817287</v>
+        <v>0.00706055105281729</v>
       </c>
       <c r="V11" s="3" t="n">
-        <v>0.3131132674055392</v>
+        <v>0.313113267405539</v>
       </c>
       <c r="W11" s="3" t="n">
-        <v>0.003004354899560139</v>
+        <v>0.00300435489956014</v>
       </c>
       <c r="X11" s="3" t="n">
-        <v>-1.841140080867862e-07</v>
+        <v>-1.84114008086786e-07</v>
       </c>
       <c r="Y11" s="3" t="n">
-        <v>1.235787831721628e-07</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1.23578783172163e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="12" s="4">
       <c r="A12" s="3" t="inlineStr">
         <is>
           <t>MSFT</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>0.1389730057390325</v>
+        <v>0.138973005739032</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>0.003915434479170364</v>
+        <v>0.00391543447917036</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.0002773664870893958</v>
+        <v>0.000277366487089396</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>0.000955647698303477</v>
@@ -2283,43 +2284,43 @@
         <v>0.00025943946452083</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>0.0004250741222480031</v>
+        <v>0.000425074122248003</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>3.516213043349495e-12</v>
+        <v>3.5162130433495e-12</v>
       </c>
       <c r="I12" s="3" t="n">
         <v>1.16054291738684e-10</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>0.0001141373920557951</v>
+        <v>0.000114137392055795</v>
       </c>
       <c r="K12" s="3" t="n">
-        <v>-0.1955330462150938</v>
+        <v>-0.195533046215094</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>0.001915457557693359</v>
+        <v>0.00191545755769336</v>
       </c>
       <c r="M12" s="3" t="n">
-        <v>-0.04485522365651801</v>
+        <v>-0.044855223656518</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>-0.003100424374661551</v>
+        <v>-0.00310042437466155</v>
       </c>
       <c r="O12" s="3" t="n">
-        <v>0.003285711662696016</v>
+        <v>0.00328571166269602</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>0.002479273888241455</v>
+        <v>0.00247927388824145</v>
       </c>
       <c r="Q12" s="3" t="n">
-        <v>0.002980278628182409</v>
+        <v>0.00298027862818241</v>
       </c>
       <c r="R12" s="3" t="n">
-        <v>0.7157011279948337</v>
+        <v>0.715701127994834</v>
       </c>
       <c r="S12" s="3" t="n">
-        <v>0.01539719178663329</v>
+        <v>0.0153971917866333</v>
       </c>
       <c r="T12" s="3" t="n">
         <v>0.00134129310717358</v>
@@ -2331,16 +2332,16 @@
         <v>0.254642921893969</v>
       </c>
       <c r="W12" s="3" t="n">
-        <v>0.003574548976889779</v>
+        <v>0.00357454897688978</v>
       </c>
       <c r="X12" s="3" t="n">
-        <v>9.620663646893958e-05</v>
+        <v>9.62066364689396e-05</v>
       </c>
       <c r="Y12" s="3" t="n">
-        <v>4.147029277220611e-07</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>4.14702927722061e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="13" s="4">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>NVDA</t>
@@ -2350,7 +2351,7 @@
         <v>0.138667176977836</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>0.01364874020995221</v>
+        <v>0.0136487402099522</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>0.00101651452774808</v>
@@ -2359,28 +2360,28 @@
         <v>0.00349467093808608</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0.0005654954565744543</v>
+        <v>0.000565495456574454</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>0.001459616471118063</v>
+        <v>0.00145961647111806</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>-1.13677188660795e-08</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>6.597513064809142e-09</v>
+        <v>6.59751306480914e-09</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>-0.0005964812927204615</v>
+        <v>-0.000596481292720461</v>
       </c>
       <c r="K13" s="3" t="n">
-        <v>-0.6881282599651679</v>
+        <v>-0.688128259965168</v>
       </c>
       <c r="L13" s="3" t="n">
         <v>-0.00500475744653891</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>-0.1824719104951031</v>
+        <v>-0.182471910495103</v>
       </c>
       <c r="N13" s="3" t="n">
         <v>-0.0155906738979146</v>
@@ -2389,19 +2390,19 @@
         <v>-0.0091037088891123</v>
       </c>
       <c r="P13" s="3" t="n">
-        <v>0.01578314848729194</v>
+        <v>0.0157831484872919</v>
       </c>
       <c r="Q13" s="3" t="n">
-        <v>0.01510439966701026</v>
+        <v>0.0151043996670103</v>
       </c>
       <c r="R13" s="3" t="n">
-        <v>0.2768802808433715</v>
+        <v>0.276880280843371</v>
       </c>
       <c r="S13" s="3" t="n">
-        <v>0.02090641865060755</v>
+        <v>0.0209064186506075</v>
       </c>
       <c r="T13" s="3" t="n">
-        <v>0.001786219784475488</v>
+        <v>0.00178621978447549</v>
       </c>
       <c r="U13" s="3" t="n">
         <v>0.0120998126495009</v>
@@ -2410,141 +2411,141 @@
         <v>0.6832892806801339</v>
       </c>
       <c r="W13" s="3" t="n">
-        <v>0.005040329967236482</v>
+        <v>0.00504032996723648</v>
       </c>
       <c r="X13" s="3" t="n">
-        <v>-2.988166290487612e-06</v>
+        <v>-2.98816629048761e-06</v>
       </c>
       <c r="Y13" s="3" t="n">
-        <v>6.455909646098714e-07</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>6.45590964609871e-07</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="14" s="4">
       <c r="A14" s="3" t="inlineStr">
         <is>
           <t>IBM</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>0.1378357862678281</v>
+        <v>0.137835786267828</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>0.00262912743357105</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>0.0002128036083618136</v>
+        <v>0.000212803608361814</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>0.0007550105453869518</v>
+        <v>0.000755010545386952</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>0.000197797988452706</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>0.0002873078345074202</v>
+        <v>0.00028730783450742</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>9.764548786378967e-10</v>
+        <v>9.764548786378971e-10</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>8.632708600256388e-10</v>
+        <v>8.63270860025639e-10</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>7.164932462630507e-06</v>
+        <v>7.16493246263051e-06</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>-0.1313568201263676</v>
+        <v>-0.131356820126368</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>0.0004122300947412933</v>
+        <v>0.000412230094741293</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>-0.03733462936682114</v>
+        <v>-0.0373346293668211</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>-0.003391007995151703</v>
+        <v>-0.0033910079951517</v>
       </c>
       <c r="O14" s="3" t="n">
-        <v>0.0006010658622721541</v>
+        <v>0.000601065862272154</v>
       </c>
       <c r="P14" s="3" t="n">
-        <v>0.001136266385262754</v>
+        <v>0.00113626638526275</v>
       </c>
       <c r="Q14" s="3" t="n">
-        <v>0.0007052452766741508</v>
+        <v>0.000705245276674151</v>
       </c>
       <c r="R14" s="3" t="n">
-        <v>0.7535866348839824</v>
+        <v>0.753586634883982</v>
       </c>
       <c r="S14" s="3" t="n">
-        <v>0.01144062926888792</v>
+        <v>0.0114406292688879</v>
       </c>
       <c r="T14" s="3" t="n">
-        <v>0.0009473196996567615</v>
+        <v>0.000947319699656761</v>
       </c>
       <c r="U14" s="3" t="n">
-        <v>0.005646096015236413</v>
+        <v>0.00564609601523641</v>
       </c>
       <c r="V14" s="3" t="n">
-        <v>0.2261926058943425</v>
+        <v>0.226192605894343</v>
       </c>
       <c r="W14" s="3" t="n">
-        <v>0.002178581659964665</v>
+        <v>0.00217858165996466</v>
       </c>
       <c r="X14" s="3" t="n">
-        <v>3.699638940796182e-06</v>
+        <v>3.69963894079618e-06</v>
       </c>
       <c r="Y14" s="3" t="n">
-        <v>4.432938988450102e-06</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>4.4329389884501e-06</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="15" s="4">
       <c r="A15" s="3" t="inlineStr">
         <is>
           <t>GOOG</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>0.1347183583006321</v>
+        <v>0.134718358300632</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>0.04205611909740369</v>
+        <v>0.0420561190974037</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>0.003274801981651106</v>
+        <v>0.00327480198165111</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>0.01106273795466514</v>
+        <v>0.0110627379546651</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>0.0016506194303711</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>0.004380404036544334</v>
+        <v>0.00438040403654433</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>8.275148316984776e-10</v>
+        <v>8.27514831698478e-10</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>1.565966441311088e-07</v>
+        <v>1.56596644131109e-07</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>0.004912426201146909</v>
+        <v>0.00491242620114691</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>-2.097658104190129</v>
+        <v>-2.09765810419013</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>-0.02174703859039384</v>
+        <v>-0.0217470385903938</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>-0.5790608407109995</v>
+        <v>-0.5790608407109989</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>-0.05048331089569011</v>
+        <v>-0.0504833108956901</v>
       </c>
       <c r="O15" s="3" t="n">
-        <v>-0.01556327402714886</v>
+        <v>-0.0155632740271489</v>
       </c>
       <c r="P15" s="3" t="n">
         <v>-0.0264748656494369</v>
@@ -2553,28 +2554,365 @@
         <v>-0.021281798332641</v>
       </c>
       <c r="R15" s="3" t="n">
-        <v>0.1351679870191684</v>
+        <v>0.135167987019168</v>
       </c>
       <c r="S15" s="3" t="n">
-        <v>0.02999827042401006</v>
+        <v>0.0299982704240101</v>
       </c>
       <c r="T15" s="3" t="n">
-        <v>0.002723150097429514</v>
+        <v>0.00272315009742951</v>
       </c>
       <c r="U15" s="3" t="n">
-        <v>0.01622218585385264</v>
+        <v>0.0162221858538526</v>
       </c>
       <c r="V15" s="3" t="n">
-        <v>0.8087608772149593</v>
+        <v>0.808760877214959</v>
       </c>
       <c r="W15" s="3" t="n">
-        <v>0.006333743460590091</v>
+        <v>0.00633374346059009</v>
       </c>
       <c r="X15" s="3" t="n">
-        <v>0.0007845346194908972</v>
+        <v>0.000784534619490897</v>
       </c>
       <c r="Y15" s="3" t="n">
-        <v>9.251310499103086e-06</v>
+        <v>9.25131049910309e-06</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:Y8"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="3" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="12.8" r="1" s="4">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Stock</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>a3</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>a5</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>a6</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>a7</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>a8</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="n"/>
+      <c r="L1" s="5" t="n"/>
+      <c r="M1" s="5" t="n"/>
+      <c r="N1" s="5" t="n"/>
+      <c r="O1" s="5" t="n"/>
+      <c r="P1" s="5" t="n"/>
+      <c r="Q1" s="5" t="n"/>
+      <c r="R1" s="5" t="n"/>
+      <c r="S1" s="5" t="n"/>
+      <c r="T1" s="5" t="n"/>
+      <c r="U1" s="5" t="n"/>
+      <c r="V1" s="5" t="n"/>
+      <c r="W1" s="5" t="n"/>
+      <c r="X1" s="5" t="n"/>
+      <c r="Y1" s="5" t="n"/>
+    </row>
+    <row customHeight="1" ht="12.8" r="2" s="4">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>NKLA</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0.01653374795259507</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>-0.01349018989072275</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0.0009910385456232483</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.002211684408468581</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0.02739243731267229</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>0.001363141302623336</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>-1.776200242619236e-08</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>-4.938997475683575e-09</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0.1395138973315981</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="4">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>-0.06427723582525341</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>-0.0007559920135603266</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>-0.0005380007220262511</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.0001724943831567084</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.000300614345162068</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0.001241520741423059</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>-1.171055494100244e-11</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>2.835877891997141e-13</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0.3100216411810126</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="4" s="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>SNE</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.01481586907528008</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.002144204037796057</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.0008992895166178896</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>-0.001594513840965123</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>-0.005059605400875675</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>-0.0004837206746742919</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>3.326766940264444e-10</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>1.507407204559867e-10</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.1143373646795085</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="5" s="4">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>-0.09077986932814923</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.004314249365721232</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>9.14569398570725e-05</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>-0.002763584435228912</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>-0.001624397435542726</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0.00180138615355606</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>2.353703671691291e-10</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>-6.818434920493999e-10</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0.3747829709688214</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="6" s="4">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>-0.0798736893367518</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.002085175407423459</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.0008591001259896575</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>-0.003265011017815574</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0.0009594642852026158</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>-4.846269218695619e-05</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>-3.715059552580937e-11</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>1.195078997564915e-10</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>0.2470382837785018</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="7" s="4">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>-0.8348128495112077</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0.02814438052328861</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.01461190710333258</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>-0.05727267042543521</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0.01042671051894129</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>0.002852393602227778</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>3.174484447524017e-09</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>5.102297081125259e-10</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>-0.7437235821239465</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="8" s="4">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>PLUG</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0.001896228157687162</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>-0.0002277820174557703</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.0001390295009680415</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>-0.001065031614760299</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0.002245457551767789</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>8.612943544500823e-05</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>1.705152273085189e-10</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>4.198998205197195e-11</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>0.03082075067600522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Records both ls and surface methods
</commit_message>
<xml_diff>
--- a/stockData.xlsx
+++ b/stockData.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="daily" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="60min" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5min" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dailySurface" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -463,10 +463,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="N1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Z14" activeCellId="0" pane="topLeft" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -600,558 +600,2105 @@
           <t>w7</t>
         </is>
       </c>
+      <c r="Z1" s="5" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="AA1" s="5" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="AB1" s="5" t="inlineStr">
+        <is>
+          <t>a3</t>
+        </is>
+      </c>
+      <c r="AC1" s="5" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="AD1" s="5" t="inlineStr">
+        <is>
+          <t>a5</t>
+        </is>
+      </c>
+      <c r="AE1" s="5" t="inlineStr">
+        <is>
+          <t>a6</t>
+        </is>
+      </c>
+      <c r="AF1" s="5" t="inlineStr">
+        <is>
+          <t>a7</t>
+        </is>
+      </c>
+      <c r="AG1" s="5" t="inlineStr">
+        <is>
+          <t>a8</t>
+        </is>
+      </c>
     </row>
-    <row r="2">
+    <row customHeight="1" ht="12.8" r="2" s="4">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>IBM</t>
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>0.1353339795254263</v>
+        <v>-0.03685771773773124</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.02311614774525422</v>
+        <v>-0.002817595643678447</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.002416155435321068</v>
+        <v>0.0001320589383486861</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.008756418689102752</v>
+        <v>-0.001575868091256668</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>-0.002386713597914154</v>
+        <v>-0.0001707820041139671</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>0.003248142567883146</v>
+        <v>0.0004837155014728715</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>1.683741890070394e-11</v>
+        <v>-6.802844204066801e-11</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.365890513733459e-10</v>
+        <v>-3.52911223044529e-10</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>7.987578806672784e-06</v>
+        <v>0.005438959620459324</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>-1.178914113291122</v>
+        <v>0.1481349012931485</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>-0.008682686874265128</v>
+        <v>0.002610360577524171</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>-0.4459318965908032</v>
+        <v>0.08784403859745028</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>0.06639658324626443</v>
+        <v>0.006668455242969584</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>-0.01219697570948368</v>
+        <v>-0.0005728613402185889</v>
       </c>
       <c r="P2" s="3" t="n">
-        <v>0.008753731320656585</v>
+        <v>0.01810828045586003</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>-0.006256505902792851</v>
+        <v>0.05206851183050814</v>
       </c>
       <c r="R2" s="3" t="n">
-        <v>0.1817201811518735</v>
+        <v>0.3810049995268447</v>
       </c>
       <c r="S2" s="3" t="n">
-        <v>0.2311367116934373</v>
+        <v>0.2169909429382607</v>
       </c>
       <c r="T2" s="3" t="n">
-        <v>0.228938436374275</v>
+        <v>-0.09640581853431093</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>0.1764903635473043</v>
+        <v>0.244430114838874</v>
       </c>
       <c r="V2" s="3" t="n">
-        <v>-0.01775379962266861</v>
+        <v>0.009777734361062907</v>
       </c>
       <c r="W2" s="3" t="n">
-        <v>0.179125441950419</v>
+        <v>-0.2054573433408424</v>
       </c>
       <c r="X2" s="3" t="n">
-        <v>0.00402048532970439</v>
+        <v>0.1249434466868105</v>
       </c>
       <c r="Y2" s="3" t="n">
-        <v>0.01632217957565525</v>
+        <v>0.3247159235233005</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-0.09077986932814923</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.004314249365721232</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>9.14569398570725e-05</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-0.002763584435228912</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-0.001624397435542726</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.00180138615355606</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>2.353703671691291e-10</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>-6.818434920493999e-10</v>
       </c>
     </row>
-    <row r="3">
+    <row customHeight="1" ht="12.8" r="3" s="4">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>NIO</t>
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>0.1385909283782561</v>
+        <v>0.04940236843182752</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.01050664818474728</v>
+        <v>0.004874956047946722</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.001176417984417368</v>
+        <v>0.0006658510531412245</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.004759879099648455</v>
+        <v>0.001320295918573152</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.009496628304978187</v>
+        <v>0.003359832712466788</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>0.001849711840304627</v>
+        <v>0.0009870337662536634</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>1.127368128607484e-10</v>
+        <v>7.063105906241019e-11</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>8.768050621303033e-11</v>
+        <v>5.928979741050014e-11</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>0.006256578361578916</v>
+        <v>0.05009332018190071</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>-0.483545571782841</v>
+        <v>-0.1849447926066939</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>0.04256289451534556</v>
+        <v>0.05742110845998643</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>-0.1676105457660406</v>
+        <v>0.002509702230777608</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>-0.2060824955672104</v>
+        <v>-0.02605368655371255</v>
       </c>
       <c r="O3" s="3" t="n">
-        <v>0.04853126607488272</v>
+        <v>0.06060707711143565</v>
       </c>
       <c r="P3" s="3" t="n">
-        <v>0.1057432012904757</v>
+        <v>0.09216722918372917</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>-0.00447976343857507</v>
+        <v>0.02117587537034843</v>
       </c>
       <c r="R3" s="3" t="n">
-        <v>0.1651425896038074</v>
+        <v>0.1234879440264581</v>
       </c>
       <c r="S3" s="3" t="n">
-        <v>0.1465595186880449</v>
+        <v>0.1428233428669331</v>
       </c>
       <c r="T3" s="3" t="n">
-        <v>0.1272481894178498</v>
+        <v>0.1514204667373756</v>
       </c>
       <c r="U3" s="3" t="n">
-        <v>0.1078130448519441</v>
+        <v>0.06351962870641699</v>
       </c>
       <c r="V3" s="3" t="n">
-        <v>0.102646633060844</v>
+        <v>0.07627017779521356</v>
       </c>
       <c r="W3" s="3" t="n">
-        <v>0.1093472911632663</v>
+        <v>0.1225503657347017</v>
       </c>
       <c r="X3" s="3" t="n">
-        <v>0.107830896961512</v>
+        <v>0.1368228059420201</v>
       </c>
       <c r="Y3" s="3" t="n">
-        <v>0.1334118362527315</v>
+        <v>0.1831052681908809</v>
+      </c>
+      <c r="Z3" s="3" t="n">
+        <v>-0.0798736893367518</v>
+      </c>
+      <c r="AA3" s="3" t="n">
+        <v>0.002085175407423459</v>
+      </c>
+      <c r="AB3" s="3" t="n">
+        <v>0.0008591001259896575</v>
+      </c>
+      <c r="AC3" s="3" t="n">
+        <v>-0.003265011017815574</v>
+      </c>
+      <c r="AD3" s="3" t="n">
+        <v>0.0009594642852026158</v>
+      </c>
+      <c r="AE3" s="3" t="n">
+        <v>-4.846269218695619e-05</v>
+      </c>
+      <c r="AF3" s="3" t="n">
+        <v>-3.715059552580937e-11</v>
+      </c>
+      <c r="AG3" s="3" t="n">
+        <v>1.195078997564915e-10</v>
       </c>
     </row>
-    <row r="4">
+    <row customHeight="1" ht="12.8" r="4" s="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>TSLA</t>
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.1501123784387246</v>
+        <v>-0.504050228824493</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.04612699993502843</v>
+        <v>-0.04851204346052285</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.004452833277145399</v>
+        <v>0.00148846321192723</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.01655896306969518</v>
+        <v>-0.02530538362744336</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0.02196792746131501</v>
+        <v>-0.0632776735090539</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>0.005992214192937989</v>
+        <v>-0.005476894027925139</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>7.583055445389367e-10</v>
+        <v>-1.489688542604253e-10</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>5.432902149686715e-10</v>
+        <v>-4.527766923593824e-10</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>0.01501284839232625</v>
+        <v>1.013097110773334</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>-2.230352892383939</v>
+        <v>2.845001815500605</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0.1585061151949421</v>
+        <v>0.2178889086293621</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>-0.6529687690722783</v>
+        <v>1.61267207047386</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>-0.2921015150100861</v>
+        <v>1.787214605120229</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>0.1659283397268095</v>
+        <v>0.3144503816190087</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>-0.2082966909096421</v>
+        <v>0.3306524070229503</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>-0.443708215485173</v>
+        <v>0.8104241086209671</v>
       </c>
       <c r="R4" s="3" t="n">
-        <v>0.225364770843834</v>
+        <v>0.541895838108161</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>0.1381882030621805</v>
+        <v>0.104084423893566</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>0.1172233139627159</v>
+        <v>-0.02806327205869142</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>0.09296147935881117</v>
+        <v>0.1018562345385133</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>0.05748897378551517</v>
+        <v>0.1185857709615736</v>
       </c>
       <c r="W4" s="3" t="n">
-        <v>0.09152875398670732</v>
+        <v>0.05991353894528866</v>
       </c>
       <c r="X4" s="3" t="n">
-        <v>0.1405952647913003</v>
+        <v>0.01981535693927166</v>
       </c>
       <c r="Y4" s="3" t="n">
-        <v>0.1366492402089356</v>
+        <v>0.0819121086723172</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>-0.8348128495112077</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.02814438052328861</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.01461190710333258</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-0.05727267042543521</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.01042671051894129</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.002852393602227778</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>3.174484447524017e-09</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>5.102297081125259e-10</v>
       </c>
     </row>
-    <row r="5">
+    <row customHeight="1" ht="12.8" r="5" s="4">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>PLUG</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.137114581169123</v>
+        <v>0.002141501337554703</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>0.08166580030685124</v>
+        <v>0.001412197835800743</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.007217073132578467</v>
+        <v>0.0001068642916901067</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.0249984170025428</v>
+        <v>-0.0002222826364134583</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>0.04954374236238585</v>
+        <v>0.002644955403886696</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>0.0106921106147825</v>
+        <v>0.0002030815516294665</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>1.586549400427411e-10</v>
+        <v>1.756059208901884e-10</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>7.741208127169423e-11</v>
+        <v>3.000121364556456e-11</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>-0.008958351860397921</v>
+        <v>0.002014770379924333</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>-3.981024836687937</v>
+        <v>-0.06541162111845809</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>0.02747215132586744</v>
+        <v>0.003747119749791333</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>-1.150648239630023</v>
+        <v>0.01269247661326678</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>-1.223808236677121</v>
+        <v>-0.06308260636678317</v>
       </c>
       <c r="O5" s="3" t="n">
-        <v>0.04442122561322988</v>
+        <v>0.004319888339646653</v>
       </c>
       <c r="P5" s="3" t="n">
-        <v>-0.02229436639244444</v>
+        <v>0.008767682809086056</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>-0.05326259367670187</v>
+        <v>-0.006891204257053372</v>
       </c>
       <c r="R5" s="3" t="n">
-        <v>0.4015410144813033</v>
+        <v>0.2858624128423747</v>
       </c>
       <c r="S5" s="3" t="n">
-        <v>0.1607060218261482</v>
+        <v>0.1269972498547989</v>
       </c>
       <c r="T5" s="3" t="n">
-        <v>0.1397617031435922</v>
+        <v>0.09457366515509519</v>
       </c>
       <c r="U5" s="3" t="n">
-        <v>0.09717623500396873</v>
+        <v>-0.0395004003421638</v>
       </c>
       <c r="V5" s="3" t="n">
-        <v>0.07650906078671398</v>
+        <v>0.1859754360236796</v>
       </c>
       <c r="W5" s="3" t="n">
-        <v>0.1151797229826008</v>
+        <v>0.09997465316576323</v>
       </c>
       <c r="X5" s="3" t="n">
-        <v>0.002569980053887135</v>
+        <v>0.1299693600297493</v>
       </c>
       <c r="Y5" s="3" t="n">
-        <v>0.006556261721785637</v>
+        <v>0.1161476232707028</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.001896228157687162</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-0.0002277820174557703</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.0001390295009680415</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-0.001065031614760299</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.002245457551767789</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>8.612943544500823e-05</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1.705152273085189e-10</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>4.198998205197195e-11</v>
       </c>
     </row>
-    <row r="6">
+    <row customHeight="1" ht="12.8" r="6" s="4">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>NKLA</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>0.1367167143397206</v>
+        <v>-0.02356754042639839</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>0.02314229710689453</v>
+        <v>0.004969432985012319</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.002204323359715545</v>
+        <v>0.0004282979206975375</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.005159682028524805</v>
+        <v>-1.898158955623247e-05</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.01701290855751802</v>
+        <v>0.01055228735097205</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>0.004072116730582306</v>
+        <v>0.0007632941694383325</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>5.884292817423834e-09</v>
+        <v>-5.966345411145286e-09</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>2.531021603109672e-10</v>
+        <v>-2.153414156582772e-09</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>-0.00394161897945279</v>
+        <v>0.0137413580788218</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>-1.287373995580736</v>
+        <v>-0.2685048955323465</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>-0.06874997834314774</v>
+        <v>-0.00518679083348693</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>-0.250303064702823</v>
+        <v>0.01136904725893157</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>-0.4513940847565958</v>
+        <v>-0.2768314380148909</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>-0.06085719663435713</v>
+        <v>-0.003140026180464402</v>
       </c>
       <c r="P6" s="3" t="n">
-        <v>0.05406108151807273</v>
+        <v>-0.0313086592059576</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>-0.001910059861398935</v>
+        <v>0.1264966369715441</v>
       </c>
       <c r="R6" s="3" t="n">
-        <v>0.2054564861933204</v>
+        <v>0.3348186245770081</v>
       </c>
       <c r="S6" s="3" t="n">
-        <v>0.1667226846709638</v>
+        <v>-0.3384507926567589</v>
       </c>
       <c r="T6" s="3" t="n">
-        <v>0.1507470459073334</v>
+        <v>-0.2768981659099114</v>
       </c>
       <c r="U6" s="3" t="n">
-        <v>0.08168630253695956</v>
+        <v>0.002868077365266145</v>
       </c>
       <c r="V6" s="3" t="n">
-        <v>0.1345216979067013</v>
+        <v>-0.788784228309241</v>
       </c>
       <c r="W6" s="3" t="n">
-        <v>0.1330197731249609</v>
+        <v>-0.2357156381327657</v>
       </c>
       <c r="X6" s="3" t="n">
-        <v>0.1127224085050003</v>
+        <v>1.081245119833169</v>
       </c>
       <c r="Y6" s="3" t="n">
-        <v>0.01512360115476023</v>
+        <v>1.220917003233234</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.01653374795259507</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>-0.01349018989072275</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.0009910385456232483</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.002211684408468581</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.02739243731267229</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.001363141302623336</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>-1.776200242619236e-08</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>-4.938997475683575e-09</v>
       </c>
     </row>
-    <row r="7">
+    <row customHeight="1" ht="12.8" r="7" s="4">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>MSFT</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.1345400174778676</v>
+        <v>-0.0541096341920435</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.01036200100409962</v>
+        <v>-0.003641222379031455</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.001119259071693009</v>
+        <v>-0.0002117839994927389</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.003971722791948849</v>
+        <v>-0.001397930774494565</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.0006543173600419557</v>
+        <v>-0.002056322346151126</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>0.001466221734135586</v>
+        <v>0.0001656120923496778</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>5.019653753372684e-12</v>
+        <v>-6.605762898345022e-12</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>3.353349052686357e-11</v>
+        <v>-1.968177567690737e-11</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>0.002384517343013836</v>
+        <v>0.03390898600149495</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>-0.5127426748859708</v>
+        <v>0.2181513253208743</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0.01702644247593209</v>
+        <v>0.029616702507322</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>-0.1745143201006574</v>
+        <v>0.09940280097300808</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>0.02079050501177461</v>
+        <v>0.07162495236910421</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>0.01951049090438907</v>
+        <v>0.0234358523486037</v>
       </c>
       <c r="P7" s="3" t="n">
-        <v>0.05828798079919199</v>
+        <v>-0.004433861379156892</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>0.06447206528427187</v>
+        <v>0.0080995803611408</v>
       </c>
       <c r="R7" s="3" t="n">
-        <v>0.2208767591637097</v>
+        <v>0.2840275743716579</v>
       </c>
       <c r="S7" s="3" t="n">
-        <v>0.1953307709446786</v>
+        <v>0.2184469750477683</v>
       </c>
       <c r="T7" s="3" t="n">
-        <v>0.201067128291379</v>
+        <v>0.1210091183397872</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>0.1539560436556384</v>
+        <v>0.1723072480026605</v>
       </c>
       <c r="V7" s="3" t="n">
-        <v>0.009620442903557196</v>
+        <v>0.09633645921112184</v>
       </c>
       <c r="W7" s="3" t="n">
-        <v>0.154354047161639</v>
+        <v>-0.05548584574744336</v>
       </c>
       <c r="X7" s="3" t="n">
-        <v>0.01815311472078176</v>
+        <v>0.0763188814437902</v>
       </c>
       <c r="Y7" s="3" t="n">
-        <v>0.04664169315861624</v>
+        <v>0.0870395893306574</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>-0.06427723582525341</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-0.0007559920135603266</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-0.0005380007220262511</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.0001724943831567084</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.000300614345162068</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.001241520741423059</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>-1.171055494100244e-11</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>2.835877891997141e-13</v>
       </c>
     </row>
-    <row r="8">
+    <row customHeight="1" ht="12.8" r="8" s="4">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>SNE</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0.1362359037010507</v>
+        <v>0.04812294061758202</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0.01429507612645025</v>
+        <v>0.006528292434123106</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.001575430175363643</v>
+        <v>0.0007691220090598657</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.005439131765689395</v>
+        <v>0.001692095985905549</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.0004191584755106373</v>
+        <v>-0.004401840135882744</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>0.002068530526622674</v>
+        <v>0.0008703536350634802</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>2.348807752275892e-10</v>
+        <v>3.591106573425146e-10</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>1.078206231965275e-09</v>
+        <v>1.160527214878017e-09</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>0.0001337265080490603</v>
+        <v>-0.02019731447660819</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>-0.7216613100202224</v>
+        <v>-0.3465323193585201</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>-0.001553549086587638</v>
+        <v>-0.01715777661188136</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>-0.2746776158112832</v>
+        <v>-0.1008198642980002</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>-0.006554733305411077</v>
+        <v>0.08651041642253654</v>
       </c>
       <c r="O8" s="3" t="n">
-        <v>-0.0009471621737110984</v>
+        <v>-0.01721461209315205</v>
       </c>
       <c r="P8" s="3" t="n">
-        <v>-0.04028419930669253</v>
+        <v>-0.07825004975081917</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>-0.03136447011002497</v>
+        <v>-0.04860117749675129</v>
       </c>
       <c r="R8" s="3" t="n">
-        <v>0.1883611222308824</v>
+        <v>0.1504144100381651</v>
       </c>
       <c r="S8" s="3" t="n">
-        <v>0.2058170513959711</v>
+        <v>0.2115744897288817</v>
       </c>
       <c r="T8" s="3" t="n">
-        <v>0.1986039076849226</v>
+        <v>0.2182611111751959</v>
       </c>
       <c r="U8" s="3" t="n">
-        <v>0.1534964713851671</v>
+        <v>0.1075773372147931</v>
       </c>
       <c r="V8" s="3" t="n">
-        <v>0.004278437920373342</v>
+        <v>-0.1012562944167314</v>
       </c>
       <c r="W8" s="3" t="n">
-        <v>0.155307547608612</v>
+        <v>0.1470940809986897</v>
       </c>
       <c r="X8" s="3" t="n">
-        <v>0.03783677720947085</v>
+        <v>0.1301952496846008</v>
       </c>
       <c r="Y8" s="3" t="n">
-        <v>0.05629868456460045</v>
+        <v>0.1361396155764051</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.01481586907528008</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.002144204037796057</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.0008992895166178896</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>-0.001594513840965123</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>-0.005059605400875675</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>-0.0004837206746742919</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>3.326766940264444e-10</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>1.507407204559867e-10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RIDE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.0993666386958106</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0004379171543120767</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.000309601733346801</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.0004479212196223649</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1.320776506969141e-05</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.229638805502424e-05</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-2.435195673364017e-09</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-4.322269980190701e-10</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.04970434143643636</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.001265933540260606</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0210489398365051</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.04571512896952831</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.02980838081116663</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.02639990750855549</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.01755394451993037</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.03507520689530996</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.8386489737975904</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-0.0899240643928004</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-0.3775989948360345</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.1441610229670474</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.003009833175451338</v>
+      </c>
+      <c r="W9" t="n">
+        <v>-0.04529758573099787</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.3780599913189392</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.1489408237008045</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-0.1300476301488365</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>-0.0001942415507129146</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.0005204863362743429</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-0.001011194219540862</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.001434044705019471</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.0006158624168364275</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-1.980140187554167e-09</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>6.090542178791217e-10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>FUV</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-0.05472797643673162</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0003093825420958424</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7.74057437494632e-05</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0008420809683314867</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.0009909824264799671</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0001575494207978359</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-2.46395291309571e-09</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6.690175046013896e-10</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.01617953583531235</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-0.003421466850933194</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.01230380345197831</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-0.02461808014284163</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.04025475347290817</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.01316054611684563</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.01156583775874782</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.001699101516890357</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-1.615104876163801</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.3146083621972154</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.7604367649414412</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1.449595932814414</v>
+      </c>
+      <c r="V10" t="n">
+        <v>-0.8299917422825385</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.8030592474813775</v>
+      </c>
+      <c r="X10" t="n">
+        <v>-1.046515485146261</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>1.163911796158153</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-0.1504972452098424</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>-0.0003687894108892968</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>-5.674572145883221e-05</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.0007641840380870556</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>-0.0009662350027916755</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.0004371811984149913</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>-7.293756793771568e-09</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>3.40225335840764e-09</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FCEL</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.0007408045831969821</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.000720540946156451</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0001023558287935293</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5.058531478858599e-05</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.003913846267021014</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0003316703202790692</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.599990040864839e-11</v>
+      </c>
+      <c r="I11" t="n">
+        <v>3.762802877337427e-11</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.003629803423480927</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-0.03735487555817642</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.001320391099898081</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-0.006150517861858352</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.089807615441849</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.0003696315753246856</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-0.002674360749791109</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-0.005574269595698077</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.291846808626768</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-0.1593104942380385</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-0.2126688565031265</v>
+      </c>
+      <c r="U11" t="n">
+        <v>-0.0218347382931187</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.7282736327803382</v>
+      </c>
+      <c r="W11" t="n">
+        <v>-0.3880024289262473</v>
+      </c>
+      <c r="X11" t="n">
+        <v>-0.02256006451761871</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>-0.2157438589289567</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-0.000985607017858637</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.002664698064723797</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>-3.909855177660401e-05</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>-0.000928293185743336</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>-0.003580747536310438</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.0007968489461046815</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>2.180324395724531e-11</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>2.263064046869857e-11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BLNK</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.05245435979547292</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.004500449461706256</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0007009136679118958</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.00295586803972132</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001243611838996613</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0007948218078886895</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4.885824905819943e-10</v>
+      </c>
+      <c r="I12" t="n">
+        <v>8.973985826782443e-10</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.04256723441679875</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-0.1637272668361864</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0572796520235539</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-0.07146390463097962</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.01746374443545767</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.06010365643033865</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.03099713500588243</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-0.1503066404496664</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.1065314800463641</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.1404723390390075</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.1785364664941053</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.1356174133582592</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.04194924244465304</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.1096436251272432</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.02503116154139152</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.262218271948976</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>-0.2469493199113309</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>-0.01242925388375943</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.001738434031036774</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>-0.002697560559684754</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.006460619521963052</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.0003612907507092597</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>4.772433024366454e-09</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>2.349041083531257e-09</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CBAT</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.02690211522730953</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.0004281572497471209</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-5.425868611448391e-05</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.0004116828312537652</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-9.816075727263508e-05</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-8.299800167386215e-05</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-5.412644563487986e-10</v>
+      </c>
+      <c r="I13" t="n">
+        <v>3.09244097703147e-11</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.001219023513038413</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.02273460197101669</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0003677457155190729</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0169520467156279</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.003989507300270047</v>
+      </c>
+      <c r="O13" t="n">
+        <v>9.497614978544394e-05</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-0.01019623461618523</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.0005057320054431408</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.3607019558947575</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.128161027268479</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0969888918051041</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.1675060622407474</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.03316227956410318</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.07648031489561107</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.1667321999535447</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>-0.02973273162234674</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>-0.02797895808597925</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.0002200841768724311</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>9.113583603856846e-06</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>-0.0004892469549767515</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>-0.0002000383026290459</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.0001174843783650428</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>-9.104132572378196e-10</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>-1.349748404448964e-10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-0.01486524405208291</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.01476785616982989</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.0007021093500898875</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.005694415167319646</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.02195094853388629</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-0.002264740072354747</v>
+      </c>
+      <c r="H14" t="n">
+        <v>9.726376366230768e-10</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.993181357328388e-09</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.6708466690670682</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.401069328784643</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.6224659705569602</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.9189102761269642</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1.150037791206968</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.6341144552524045</v>
+      </c>
+      <c r="P14" t="n">
+        <v>-0.2752686699340866</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-0.5295635848339084</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-0.5936853266116513</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-0.396519521611096</v>
+      </c>
+      <c r="T14" t="n">
+        <v>-0.1755097832506744</v>
+      </c>
+      <c r="U14" t="n">
+        <v>-0.3021066976144631</v>
+      </c>
+      <c r="V14" t="n">
+        <v>-0.4511837281324789</v>
+      </c>
+      <c r="W14" t="n">
+        <v>-0.3235446521638817</v>
+      </c>
+      <c r="X14" t="n">
+        <v>1.536256262219553</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>1.706293447164693</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>-0.03205551607680336</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>-0.005956269669566779</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0.00144423683650702</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>-0.007177963486478553</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>-0.01026437585921658</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>-0.001171926455534823</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>-1.400480449436565e-09</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>5.144159342037757e-09</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-0.7595710618593282</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.01585066418546302</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.0005195838002604999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.002116486743897736</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.03003559627828112</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.001349124155467507</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-1.305183689506533e-12</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-6.553476436790184e-13</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.128745211767862</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.8826561407014151</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.02066879367755551</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.1261374999451069</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.8019611905530514</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.03026039308196496</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.06612163408551165</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.05031907371274774</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.4117709772696416</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.1507939534586172</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.04225466765213376</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.03776598309409358</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.2424494258854562</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.0649090360954908</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.0311322282298976</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.01892372831466918</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>-0.8401959318119073</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0.007683874957744845</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>-0.0007657789360288736</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0.00307138575735243</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>-0.02412185816764734</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.001838346919314561</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>-2.401726255053141e-12</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>4.414392595303401e-12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.009557957179367471</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.001955625010117703</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-9.7957344240074e-05</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.001080457794420291</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.009694859488805933</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.0003777374540583942</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2.313177403370592e-10</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.446689533341446e-10</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.08405165625626156</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.1936764750546699</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.09111678827477425</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.1493106072292791</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.3325573123079658</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.09362837468608318</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.118346083301792</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-0.08459603877209362</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.3456203271044367</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-0.2571023040408118</v>
+      </c>
+      <c r="T16" t="n">
+        <v>-0.1117023198398381</v>
+      </c>
+      <c r="U16" t="n">
+        <v>-0.2720184342635151</v>
+      </c>
+      <c r="V16" t="n">
+        <v>-1.001164760451098</v>
+      </c>
+      <c r="W16" t="n">
+        <v>-0.253489652316866</v>
+      </c>
+      <c r="X16" t="n">
+        <v>1.182801125333293</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1.367056018474399</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>-0.005430344965952611</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0.004484172742779801</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>8.6275186778903e-05</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>-0.001917570529813</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>-0.008014016338686545</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>-0.0009112731699334378</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>7.910117231540626e-11</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>1.372073061783218e-10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ZM</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.02232679991000623</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.01504009117117437</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.002798022263603238</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.01193402528470811</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.007001338794368834</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0005719205662411794</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.032151822599528e-09</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-2.149701530137419e-09</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.5579426321935922</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-0.1704926983617752</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.7448329408392126</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1.32929829702942</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.8904145043512961</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.6528627849070179</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.6058262540951311</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1.020374075110579</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-0.8983789186100858</v>
+      </c>
+      <c r="S17" t="n">
+        <v>-0.5938712782381678</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.9756329671427656</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.8478133689657913</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.2323570830413114</v>
+      </c>
+      <c r="W17" t="n">
+        <v>-0.1110980504924805</v>
+      </c>
+      <c r="X17" t="n">
+        <v>-0.3677473337284564</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.9152921619193223</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>-0.1060315547936568</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0.1879950640168573</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>-0.01472300841972481</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>-0.02810485425285736</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.07682431890319877</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.0002472999766014057</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>1.551080752501217e-07</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>-1.308670173596553e-07</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.03404535615530571</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.01174487341913565</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.001058581569367479</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.005804130579984887</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.007566945398122067</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-0.001492327183217618</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2.470735182409393e-11</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.933407068099997e-11</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.1422670800280446</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.7528691068315765</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.1408208651753759</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.4378846819163144</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.2965449954541609</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.1393020007692248</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.1026275293414777</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.04392080973698253</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.1659831238595774</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.2276150214775976</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.1944380751467482</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.2233142465927237</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.121722636804464</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.1538432108167743</v>
+      </c>
+      <c r="X18" t="n">
+        <v>-0.03722105098200737</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>-0.04969526371587793</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>-0.03091108771865475</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0.004908872847024788</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>-0.000570596860283093</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>-0.004275163472051203</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>-0.00536604933892512</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>3.198160631671987e-05</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>-9.059723449244499e-11</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>7.982747141562392e-11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PYPL</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.00378277511764066</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.008890023557566455</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.0006246160163651917</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.002346155075171631</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-0.000632240076549424</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-0.0003433417002995782</v>
+      </c>
+      <c r="H19" t="n">
+        <v>5.322720487113349e-10</v>
+      </c>
+      <c r="I19" t="n">
+        <v>3.558923383821463e-10</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.1496699226973211</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.6328782095968885</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.1611763554746141</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.2770543149129651</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.1609838936769638</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.149469120759847</v>
+      </c>
+      <c r="P19" t="n">
+        <v>-0.0220548367196602</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.06695843431283097</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.1769712929149521</v>
+      </c>
+      <c r="S19" t="n">
+        <v>2.050791849487771</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1.385447305842023</v>
+      </c>
+      <c r="U19" t="n">
+        <v>1.087021636438844</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.1402721651262568</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.4402233173841041</v>
+      </c>
+      <c r="X19" t="n">
+        <v>-2.354135057941545</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>-1.926592509252407</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>-0.01690470643794151</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>-0.007261421065676399</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>-0.00105424336865475</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0.002855828999091077</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0.002589735379812048</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.001204728793136837</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>1.509585207236937e-09</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>-6.646928671352629e-10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CRM</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.06285013447373433</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.005482418698714316</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.0004049028267868442</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.00409689256452437</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.0004343715079604331</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-0.0006285180832380942</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.277508536421655e-11</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-5.029575131300361e-11</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.07594725246148067</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.3445229213246455</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.05728968007831569</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.2736795029283018</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.06130314201961563</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.05808691929433249</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.03707818016779759</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.05414902933197601</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.3173095959243771</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.1715622311576986</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.1237437133385348</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.2581833815010237</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.01050860861167822</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.1098997643477067</v>
+      </c>
+      <c r="X20" t="n">
+        <v>-0.01889550046413116</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.02768820558311183</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>-0.07391164579112842</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0.00518338519136685</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0.0002723125630655285</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>-0.005460813751905188</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.0007311193767487801</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.0001894862953042732</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>7.934219894565895e-11</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>-3.520369605947825e-11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.02522842619594725</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.00113167297058762</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4.897078916784776e-05</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.0005865711854506852</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0009816571290013247</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0002169079232118153</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-6.199491142695102e-12</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2.441940521692278e-11</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.008985588689732824</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-0.04575911036526324</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.01157095647890701</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.04135681364414839</v>
+      </c>
+      <c r="N21" t="n">
+        <v>-0.01348449695579261</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.01088206341003708</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.007603350953939745</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-0.0006496606360798606</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.2701019745439703</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.1798373917644937</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.06534574319758023</v>
+      </c>
+      <c r="U21" t="n">
+        <v>-0.1683394783708058</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.1261144257476843</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0.1673498095682235</v>
+      </c>
+      <c r="X21" t="n">
+        <v>-0.05962532308649571</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0.4192154566353494</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.005649743894742789</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0.0009788451157530039</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0.0001718591781633888</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>-0.001991961348784928</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.001083641878709564</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.0001299803666477991</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>-1.891081074770585e-11</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>2.610250557222141e-11</v>
       </c>
     </row>
   </sheetData>
@@ -1175,10 +2722,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="S1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Z1" activeCellId="0" pane="topLeft" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -1310,6 +2857,46 @@
       <c r="Y1" s="5" t="inlineStr">
         <is>
           <t>w7</t>
+        </is>
+      </c>
+      <c r="Z1" s="5" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="AA1" s="5" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="AB1" s="5" t="inlineStr">
+        <is>
+          <t>a3</t>
+        </is>
+      </c>
+      <c r="AC1" s="5" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="AD1" s="5" t="inlineStr">
+        <is>
+          <t>a5</t>
+        </is>
+      </c>
+      <c r="AE1" s="5" t="inlineStr">
+        <is>
+          <t>a6</t>
+        </is>
+      </c>
+      <c r="AF1" s="5" t="inlineStr">
+        <is>
+          <t>a7</t>
+        </is>
+      </c>
+      <c r="AG1" s="5" t="inlineStr">
+        <is>
+          <t>a8</t>
         </is>
       </c>
     </row>
@@ -1334,10 +2921,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="W1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Z27" activeCellId="0" pane="topLeft" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -1469,6 +3056,46 @@
       <c r="Y1" s="5" t="inlineStr">
         <is>
           <t>w7</t>
+        </is>
+      </c>
+      <c r="Z1" s="5" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="AA1" s="5" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="AB1" s="5" t="inlineStr">
+        <is>
+          <t>a3</t>
+        </is>
+      </c>
+      <c r="AC1" s="5" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="AD1" s="5" t="inlineStr">
+        <is>
+          <t>a5</t>
+        </is>
+      </c>
+      <c r="AE1" s="5" t="inlineStr">
+        <is>
+          <t>a6</t>
+        </is>
+      </c>
+      <c r="AF1" s="5" t="inlineStr">
+        <is>
+          <t>a7</t>
+        </is>
+      </c>
+      <c r="AG1" s="5" t="inlineStr">
+        <is>
+          <t>a8</t>
         </is>
       </c>
     </row>
@@ -2602,7 +4229,7 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -2684,31 +4311,31 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>0.01653374795259507</v>
+        <v>0.0198864807539176</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>-0.01349018989072275</v>
+        <v>-0.015971897080377</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.0009910385456232483</v>
+        <v>0.00115531966242257</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.002211684408468581</v>
+        <v>0.00216973121640974</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0.02739243731267229</v>
+        <v>0.0273889591487733</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>0.001363141302623336</v>
+        <v>0.0014271575130096</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>-1.776200242619236e-08</v>
+        <v>-1.77615237196214e-08</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>-4.938997475683575e-09</v>
+        <v>-5.0032533248577e-09</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>0.1395138973315981</v>
+        <v>0.139513897331598</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="3" s="4">
@@ -2718,31 +4345,31 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>-0.06427723582525341</v>
+        <v>-0.0493608938922811</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>-0.0007559920135603266</v>
+        <v>-0.00612027137991557</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>-0.0005380007220262511</v>
+        <v>-0.000164850523355552</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.0001724943831567084</v>
+        <v>-0.000221095290818279</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.000300614345162068</v>
+        <v>0.000211477606989875</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>0.001241520741423059</v>
+        <v>0.00145764183581373</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>-1.171055494100244e-11</v>
+        <v>-9.89232748193689e-12</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>2.835877891997141e-13</v>
+        <v>4.59731323579505e-12</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>0.3100216411810126</v>
+        <v>0.310021641181013</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="4" s="4">
@@ -2752,31 +4379,31 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.01481586907528008</v>
+        <v>0.0226150108156243</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.002144204037796057</v>
+        <v>0.000155579870261063</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.0008992895166178896</v>
+        <v>0.00103492016798735</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>-0.001594513840965123</v>
+        <v>-0.0017085434277009</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>-0.005059605400875675</v>
+        <v>-0.00533501924677903</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>-0.0004837206746742919</v>
+        <v>-0.000414797189553799</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>3.326766940264444e-10</v>
+        <v>3.20152837111504e-10</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.507407204559867e-10</v>
+        <v>1.92796195146511e-10</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>0.1143373646795085</v>
+        <v>0.114337364679509</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="5" s="4">
@@ -2786,31 +4413,31 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>-0.09077986932814923</v>
+        <v>-0.0624801485075109</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>0.004314249365721232</v>
+        <v>-0.00280368135467533</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>9.14569398570725e-05</v>
+        <v>0.0005295173082855</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>-0.002763584435228912</v>
+        <v>-0.00296285764826821</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>-0.001624397435542726</v>
+        <v>-0.0016842730924516</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>0.00180138615355606</v>
+        <v>0.00182684179451468</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>2.353703671691291e-10</v>
+        <v>2.12254314606921e-10</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>-6.818434920493999e-10</v>
+        <v>-6.49017594810553e-10</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>0.3747829709688214</v>
+        <v>0.374782970968821</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="6" s="4">
@@ -2820,31 +4447,31 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>-0.0798736893367518</v>
+        <v>-0.0571273040465563</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>0.002085175407423459</v>
+        <v>-0.0018281743272817</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.0008591001259896575</v>
+        <v>0.00117233015698008</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>-0.003265011017815574</v>
+        <v>-0.00364874801901066</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.0009594642852026158</v>
+        <v>-0.0005600959059326751</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>-4.846269218695619e-05</v>
+        <v>0.000158532958063364</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>-3.715059552580937e-11</v>
+        <v>-4.23053330565598e-11</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>1.195078997564915e-10</v>
+        <v>1.23621083507717e-10</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>0.2470382837785018</v>
+        <v>0.247038283778502</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="7" s="4">
@@ -2854,31 +4481,31 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>-0.8348128495112077</v>
+        <v>-0.841431858842933</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.02814438052328861</v>
+        <v>0.0414350993238307</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.01461190710333258</v>
+        <v>0.0135607776650021</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>-0.05727267042543521</v>
+        <v>-0.0560062774248135</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.01042671051894129</v>
+        <v>0.00904549208932968</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>0.002852393602227778</v>
+        <v>0.00217629464554853</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>3.174484447524017e-09</v>
+        <v>3.17542348935934e-09</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>5.102297081125259e-10</v>
+        <v>5.2954041386622e-10</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>-0.7437235821239465</v>
+        <v>-0.743723582123947</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="8" s="4">
@@ -2888,31 +4515,31 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0.001896228157687162</v>
+        <v>0.00194803902467811</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>-0.0002277820174557703</v>
+        <v>-0.000729153268092333</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.0001390295009680415</v>
+        <v>0.000176680778387285</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>-0.001065031614760299</v>
+        <v>-0.00112395345256183</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.002245457551767789</v>
+        <v>0.00211704271437484</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>8.612943544500823e-05</v>
+        <v>0.000111880248970907</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>1.705152273085189e-10</v>
+        <v>1.78636922569301e-10</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>4.198998205197195e-11</v>
+        <v>4.28086323173473e-11</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>0.03082075067600522</v>
+        <v>0.0308207506760052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>